<commit_message>
Kitchen AI Level 3: aliases, grocery lists, inventory reports, downloads
</commit_message>
<xml_diff>
--- a/data/exports/ingredients_dinner_week3.xlsx
+++ b/data/exports/ingredients_dinner_week3.xlsx
@@ -25,7 +25,7 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Count</t>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="5" max="5" width="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>